<commit_message>
cm: oncho add oncho forms
</commit_message>
<xml_diff>
--- a/ONCHO/Impact Assessments/Cameroon/cm_oncho_pre_stop_2_202309_couverture.xlsx
+++ b/ONCHO/Impact Assessments/Cameroon/cm_oncho_pre_stop_2_202309_couverture.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bonhe\Repositories\dsa-forms\ONCHO\Impact Assessments\Cameroon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\ONCHO\Impact Assessments\Cameroon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB9DD7C4-E28A-4521-B39A-1C29CE1491CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE938061-1528-4E57-8CA7-8FDC6CC988D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="75" yWindow="5295" windowWidth="27195" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="83">
   <si>
     <t>type</t>
   </si>
@@ -158,12 +158,6 @@
     <t xml:space="preserve">Si jamais traité ou traité de temps à autre, énoncer les raisons de non compliance </t>
   </si>
   <si>
-    <t>cm_oncho_pre_stop_2_202309_couverture</t>
-  </si>
-  <si>
-    <t>(Sept 2023) ONCHO - 2.Formulaire Couverture</t>
-  </si>
-  <si>
     <t>p_recorder_id</t>
   </si>
   <si>
@@ -270,6 +264,24 @@
   </si>
   <si>
     <t>appearance</t>
+  </si>
+  <si>
+    <t>(Sept 2023) ONCHO - 2.Formulaire Couverture V1.1</t>
+  </si>
+  <si>
+    <t>cm_oncho_pre_stop_2_202309_couverture_v1_1</t>
+  </si>
+  <si>
+    <t>p_region</t>
+  </si>
+  <si>
+    <t>p_district</t>
+  </si>
+  <si>
+    <t>Région</t>
+  </si>
+  <si>
+    <t>District</t>
   </si>
 </sst>
 </file>
@@ -682,13 +694,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L42"/>
+  <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F1" sqref="F1:G1048576"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,7 +732,7 @@
         <v>21</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>3</v>
@@ -749,10 +761,10 @@
         <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>15</v>
@@ -763,10 +775,10 @@
         <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>15</v>
@@ -777,10 +789,10 @@
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>26</v>
+        <v>82</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>15</v>
@@ -791,10 +803,10 @@
         <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>15</v>
@@ -805,26 +817,25 @@
         <v>9</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>48</v>
+      <c r="B7" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="9"/>
+        <v>20</v>
+      </c>
       <c r="H7" s="7" t="s">
         <v>15</v>
       </c>
@@ -833,39 +844,40 @@
       <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>49</v>
+      <c r="B8" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>30</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="E9" s="9"/>
       <c r="H9" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>15</v>
@@ -873,19 +885,13 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>67</v>
+        <v>30</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>15</v>
@@ -893,130 +899,164 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H12" s="7"/>
-    </row>
-    <row r="13" spans="1:12" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
+        <v>31</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>15</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" spans="1:12" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="B18" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H16" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" s="4" t="s">
+      <c r="H18" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="7" t="s">
+      <c r="C19" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D17" s="7"/>
-      <c r="H17" s="7"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="33" spans="5:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E33" s="9"/>
-    </row>
-    <row r="36" spans="5:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E36" s="10"/>
-    </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E42" s="7"/>
+    </row>
+    <row r="35" spans="5:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E35" s="9"/>
+    </row>
+    <row r="38" spans="5:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E38" s="10"/>
+    </row>
+    <row r="44" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E44" s="7"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
@@ -1062,7 +1102,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>11</v>
@@ -1073,7 +1113,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>12</v>
@@ -1090,7 +1130,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1101,7 +1141,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1112,7 +1152,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1123,7 +1163,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1134,12 +1174,12 @@
         <v>9</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B9" s="4">
         <v>2017</v>
@@ -1150,7 +1190,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B10" s="4">
         <v>2018</v>
@@ -1161,7 +1201,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B11" s="4">
         <v>2019</v>
@@ -1172,7 +1212,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B12" s="4">
         <v>2020</v>
@@ -1183,7 +1223,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B13" s="4">
         <v>2021</v>
@@ -1194,7 +1234,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B14" s="4">
         <v>2022</v>
@@ -1205,7 +1245,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B15" s="4">
         <v>2023</v>
@@ -1234,7 +1274,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1256,10 +1296,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>19</v>

</xml_diff>